<commit_message>
fixed #357 FlixelRL-357 封印状態の実装
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>&lt;val1&gt;は無敵になった</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;は巻物と杖が使えなくなった</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;は特殊攻撃が使えなくなった</t>
   </si>
   <si>
     <t>ダミー</t>
@@ -2158,7 +2164,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
@@ -2166,7 +2172,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
@@ -2174,7 +2180,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
@@ -2182,7 +2188,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
@@ -2190,7 +2196,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
@@ -2198,7 +2204,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
@@ -2206,7 +2212,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
@@ -2214,7 +2220,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
@@ -2222,7 +2228,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
@@ -2230,7 +2236,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
@@ -2238,7 +2244,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
@@ -2246,7 +2252,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
@@ -2254,7 +2260,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
@@ -2262,7 +2268,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
@@ -2270,7 +2276,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
@@ -2278,7 +2284,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
@@ -2286,7 +2292,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
@@ -2294,7 +2300,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
@@ -2302,7 +2308,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
@@ -2310,7 +2316,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
@@ -2318,7 +2324,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" ht="20" customHeight="1">
@@ -2326,7 +2332,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" ht="20" customHeight="1">
@@ -2334,7 +2340,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
@@ -2342,7 +2348,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
@@ -2350,7 +2356,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" ht="20" customHeight="1">
@@ -2358,7 +2364,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" ht="20" customHeight="1">
@@ -2366,7 +2372,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" ht="20" customHeight="1">
@@ -2374,7 +2380,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" ht="20" customHeight="1">
@@ -2382,7 +2388,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" ht="20" customHeight="1">
@@ -2390,7 +2396,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" ht="20" customHeight="1">
@@ -2398,7 +2404,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" ht="20" customHeight="1">
@@ -2406,7 +2412,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
@@ -2414,7 +2420,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
@@ -2422,7 +2428,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
@@ -2430,7 +2436,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
@@ -2438,7 +2444,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2487,7 +2493,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2495,7 +2501,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2503,7 +2509,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2511,7 +2517,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2519,7 +2525,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2527,7 +2533,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2535,7 +2541,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2543,7 +2549,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2551,7 +2557,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2559,7 +2565,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2567,7 +2573,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -2575,7 +2581,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -2583,7 +2589,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -2591,7 +2597,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -2599,7 +2605,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -2607,7 +2613,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2615,7 +2621,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -2623,7 +2629,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -2631,7 +2637,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -2639,7 +2645,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -2647,7 +2653,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -2655,7 +2661,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -2663,7 +2669,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -2671,7 +2677,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -2679,7 +2685,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -2687,7 +2693,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -2695,7 +2701,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -2703,7 +2709,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -2711,7 +2717,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -2719,7 +2725,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -2727,7 +2733,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -2735,7 +2741,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -2743,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -2751,7 +2757,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -2759,7 +2765,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
@@ -2767,7 +2773,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" ht="20" customHeight="1">
@@ -2775,7 +2781,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s" s="4">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" ht="20" customHeight="1">
@@ -2783,7 +2789,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
@@ -2791,7 +2797,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s" s="4">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -2799,7 +2805,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s" s="4">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" ht="20" customHeight="1">
@@ -2807,7 +2813,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
@@ -2815,7 +2821,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
@@ -2823,7 +2829,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" ht="20" customHeight="1">
@@ -2831,7 +2837,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s" s="4">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" ht="20" customHeight="1">
@@ -2839,7 +2845,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s" s="4">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" ht="20" customHeight="1">
@@ -2847,7 +2853,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s" s="4">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" ht="20" customHeight="1">
@@ -2855,7 +2861,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s" s="4">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
@@ -2863,7 +2869,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s" s="4">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
@@ -2871,7 +2877,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s" s="4">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
@@ -2879,7 +2885,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s" s="4">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
@@ -2887,7 +2893,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
@@ -2895,7 +2901,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s" s="4">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
@@ -2903,7 +2909,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s" s="4">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
@@ -2911,7 +2917,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s" s="4">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
@@ -2919,7 +2925,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s" s="4">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
@@ -2927,7 +2933,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
@@ -2935,7 +2941,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
@@ -2943,7 +2949,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s" s="4">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
@@ -2951,7 +2957,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s" s="4">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
@@ -2959,7 +2965,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
@@ -2967,7 +2973,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s" s="4">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
@@ -2975,7 +2981,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
@@ -2983,7 +2989,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
@@ -2991,7 +2997,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #664 FlixelRL-664 ギミックの設置
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -292,7 +292,7 @@
     <t>チュートリアルメッセージ5</t>
   </si>
   <si>
-    <t>チュートリアルメッセージ6</t>
+    <t>ブロックは攻撃すると壊すことができます</t>
   </si>
   <si>
     <t>チュートリアルメッセージ7</t>
@@ -304,7 +304,7 @@
     <t>チュートリアルメッセージ9</t>
   </si>
   <si>
-    <t>チュートリアルメッセージ10</t>
+    <t>矢印は反対方向から侵入することができません</t>
   </si>
   <si>
     <t>チュートリアルメッセージ11</t>
@@ -316,7 +316,7 @@
     <t>チュートリアルメッセージ13</t>
   </si>
   <si>
-    <t>チュートリアルメッセージ14</t>
+    <t>扉は一定数敵を倒すと開きます</t>
   </si>
   <si>
     <t>チュートリアルメッセージ15</t>

</xml_diff>

<commit_message>
fixed #602 FlixelRL-602 スタッフロール
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -12,12 +12,13 @@
     <sheet name="nameentry" sheetId="4" r:id="rId7"/>
     <sheet name="title" sheetId="5" r:id="rId8"/>
     <sheet name="deathtype" sheetId="6" r:id="rId9"/>
+    <sheet name="staffroll" sheetId="7" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="190">
   <si>
     <t>id</t>
   </si>
@@ -515,6 +516,134 @@
   </si>
   <si>
     <t>毒のダメージで力尽きた</t>
+  </si>
+  <si>
+    <t>スタッフ</t>
+  </si>
+  <si>
+    <t>ゲームデザイン：　しゅん</t>
+  </si>
+  <si>
+    <t>キャラクターデザイン：　炎堂たつや</t>
+  </si>
+  <si>
+    <t>キャラクタードット絵：　MAKIさん</t>
+  </si>
+  <si>
+    <t>アイテムドット絵：　しゅん</t>
+  </si>
+  <si>
+    <t>ダンジョンチップ：　炎堂たつや</t>
+  </si>
+  <si>
+    <t>　　　　　　　　　　しゅん</t>
+  </si>
+  <si>
+    <t>UIデザイン：　しゅん</t>
+  </si>
+  <si>
+    <t>イベント画像：　しゅん</t>
+  </si>
+  <si>
+    <t>リザルト画像：　炎堂たつや</t>
+  </si>
+  <si>
+    <t>画像素材提供</t>
+  </si>
+  <si>
+    <t>モンスタードット絵：　DENZI様</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>「DENZI部屋」</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>http://www3.wind.ne.jp/DENZI/diary/</t>
+    </r>
+  </si>
+  <si>
+    <t>イベントチップ：　ぴぽや様</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>「ぴぽや」</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>http://piposozai.blog76.fc2.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>プログラム：　しゅん</t>
+  </si>
+  <si>
+    <t>サウンド：　しゅん</t>
+  </si>
+  <si>
+    <t>シナリオ：　炎堂たつや</t>
+  </si>
+  <si>
+    <t>　　　　　　しゅん</t>
+  </si>
+  <si>
+    <t>テストプレイ：　しゅん</t>
+  </si>
+  <si>
+    <t>　　　　　　　　炎堂たつや</t>
+  </si>
+  <si>
+    <t>　　　　　　　　ANDOさん</t>
+  </si>
+  <si>
+    <t>　　　　　　　　TAKIさん</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>制作：　</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="ヒラギノ角ゴ ProN W3"/>
+      </rPr>
+      <t>2dgames.jp</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -524,7 +653,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -553,6 +682,12 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="11"/>
       <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
   </fonts>
@@ -605,7 +740,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -636,6 +771,12 @@
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,6 +796,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -3740,4 +3882,350 @@
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="42.25" style="10" customWidth="1"/>
+    <col min="3" max="256" width="12.25" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="14.95" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s" s="4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11"/>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s" s="4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s" s="4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s" s="4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" ht="20" customHeight="1">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s" s="4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s" s="4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s" s="4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s" s="4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" ht="20" customHeight="1">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" ht="20" customHeight="1">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" ht="20" customHeight="1">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" ht="20" customHeight="1">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" ht="20" customHeight="1">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" ht="20" customHeight="1">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" ht="20" customHeight="1">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" ht="20" customHeight="1">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" ht="20" customHeight="1">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s" s="4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s" s="4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="11"/>
+    </row>
+    <row r="41" ht="20" customHeight="1">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="11"/>
+    </row>
+    <row r="42" ht="20" customHeight="1">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="11"/>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" ht="20" customHeight="1">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s" s="4">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="B23" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="B44" r:id="rId3" location="" tooltip="" display=""/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed #741 FlixelRL-741 STATSの説明ポップアップ表示
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -11,15 +11,16 @@
     <sheet name="hint" sheetId="3" r:id="rId6"/>
     <sheet name="nameentry" sheetId="4" r:id="rId7"/>
     <sheet name="title" sheetId="5" r:id="rId8"/>
-    <sheet name="deathtype" sheetId="6" r:id="rId9"/>
-    <sheet name="staffroll" sheetId="7" r:id="rId10"/>
-    <sheet name="statistics" sheetId="8" r:id="rId11"/>
+    <sheet name="stats" sheetId="6" r:id="rId9"/>
+    <sheet name="deathtype" sheetId="7" r:id="rId10"/>
+    <sheet name="staffroll" sheetId="8" r:id="rId11"/>
+    <sheet name="statistics" sheetId="9" r:id="rId12"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="209">
   <si>
     <t>id</t>
   </si>
@@ -511,6 +512,21 @@
   </si>
   <si>
     <t>ゲームプレイの情報を見ます</t>
+  </si>
+  <si>
+    <t>プレイ情報を見ます</t>
+  </si>
+  <si>
+    <t>実績データを閲覧します</t>
+  </si>
+  <si>
+    <t>ゲームプレイ履歴を見ます</t>
+  </si>
+  <si>
+    <t>倒した敵の情報を見ます</t>
+  </si>
+  <si>
+    <t>獲得したアイテムを見ます</t>
   </si>
   <si>
     <t>ゲームクリア</t>
@@ -783,7 +799,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -797,6 +813,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -3926,7 +3945,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3943,7 +3962,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3975,41 +3994,130 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" t="s" s="4">
+        <v>170</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" t="s" s="4">
+        <v>171</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" t="s" s="4">
+        <v>173</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>172</v>
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2.5" style="11" customWidth="1"/>
+    <col min="2" max="2" width="42.25" style="11" customWidth="1"/>
+    <col min="3" max="256" width="12.25" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="14.95" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s" s="4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s" s="4">
+        <v>177</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -4017,7 +4125,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -4025,7 +4133,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -4033,7 +4141,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -4041,7 +4149,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -4049,7 +4157,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -4057,27 +4165,27 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="12"/>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="12"/>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -4085,7 +4193,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -4093,7 +4201,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -4101,7 +4209,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -4109,47 +4217,47 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="12"/>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="12"/>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="11"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="12"/>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -4157,33 +4265,33 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="3">
         <v>27</v>
       </c>
-      <c r="B29" s="11"/>
+      <c r="B29" s="12"/>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="3">
         <v>28</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="12"/>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="3">
         <v>29</v>
       </c>
-      <c r="B31" s="11"/>
+      <c r="B31" s="12"/>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -4191,7 +4299,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -4199,7 +4307,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -4207,71 +4315,71 @@
         <v>33</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="3">
         <v>34</v>
       </c>
-      <c r="B36" s="11"/>
+      <c r="B36" s="12"/>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="3">
         <v>35</v>
       </c>
-      <c r="B37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="3">
         <v>36</v>
       </c>
-      <c r="B38" s="11"/>
+      <c r="B38" s="12"/>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="3">
         <v>37</v>
       </c>
-      <c r="B39" s="11"/>
+      <c r="B39" s="12"/>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="3">
         <v>39</v>
       </c>
-      <c r="B41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="3">
         <v>40</v>
       </c>
-      <c r="B42" s="11"/>
+      <c r="B42" s="12"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="3">
         <v>41</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="12"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="3">
         <v>42</v>
       </c>
-      <c r="B44" s="11"/>
+      <c r="B44" s="12"/>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="3">
         <v>43</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4288,7 +4396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4299,9 +4407,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="12" customWidth="1"/>
-    <col min="2" max="2" width="42.25" style="12" customWidth="1"/>
-    <col min="3" max="256" width="12.25" style="12" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="42.25" style="13" customWidth="1"/>
+    <col min="3" max="256" width="12.25" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -4325,7 +4433,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -4333,7 +4441,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -4341,7 +4449,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -4349,7 +4457,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -4357,7 +4465,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -4365,7 +4473,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -4373,7 +4481,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -4381,7 +4489,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -4389,7 +4497,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -4397,7 +4505,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -4405,7 +4513,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>